<commit_message>
Numerous chages to make use of Python 3 and convert commands from argparse to click
</commit_message>
<xml_diff>
--- a/docs/ExampleDocument.xlsx
+++ b/docs/ExampleDocument.xlsx
@@ -1,16 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvincent/work/g2gtools/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FD6550-6A1F-3D4E-BB33-3805A610C242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="2660" windowWidth="33940" windowHeight="15200" tabRatio="500"/>
+    <workbookView xWindow="14000" yWindow="760" windowWidth="20560" windowHeight="20520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="40">
   <si>
     <t>A</t>
   </si>
@@ -76,13 +94,76 @@
   </si>
   <si>
     <t>0 based location return</t>
+  </si>
+  <si>
+    <t>1       3007272 GCC     .       CC      3007274</t>
+  </si>
+  <si>
+    <t>1       3028957 A       .       G       21683</t>
+  </si>
+  <si>
+    <t>1       3043837 .       A       G       .</t>
+  </si>
+  <si>
+    <t>1       3051722 TTTCCTTCC       .       TTCC    22773</t>
+  </si>
+  <si>
+    <t>REF</t>
+  </si>
+  <si>
+    <t>AJ</t>
+  </si>
+  <si>
+    <t>TGCCCCCCCCCCTTTTTGTG</t>
+  </si>
+  <si>
+    <t>1       3054917 G       C       .       3187</t>
+  </si>
+  <si>
+    <t>SNP</t>
+  </si>
+  <si>
+    <t>INS</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>GCC</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>TTTCCTTCC</t>
+  </si>
+  <si>
+    <t>TTCC</t>
+  </si>
+  <si>
+    <t>REVERSE</t>
+  </si>
+  <si>
+    <t>FRAG</t>
+  </si>
+  <si>
+    <t>SHARE</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>CHROM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,8 +201,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,7 +378,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -296,8 +397,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -382,6 +487,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -402,7 +515,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Left Bracket 2"/>
+        <xdr:cNvPr id="3" name="Left Bracket 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -456,7 +575,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Left Bracket 3"/>
+        <xdr:cNvPr id="4" name="Left Bracket 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -510,7 +635,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Left Bracket 4"/>
+        <xdr:cNvPr id="5" name="Left Bracket 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -564,7 +695,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Left Bracket 5"/>
+        <xdr:cNvPr id="6" name="Left Bracket 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -618,7 +755,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Left Bracket 6"/>
+        <xdr:cNvPr id="7" name="Left Bracket 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -981,14 +1124,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="2.6640625" customWidth="1"/>
     <col min="7" max="7" width="2.6640625" customWidth="1"/>
@@ -998,7 +1141,7 @@
     <col min="16" max="16" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F1" t="s">
         <v>17</v>
       </c>
@@ -1012,22 +1155,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
@@ -1054,13 +1197,13 @@
       </c>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="Q13" s="7"/>
       <c r="R13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>3000019</v>
       </c>
@@ -1095,7 +1238,7 @@
         <v>3000021</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>3003197</v>
       </c>
@@ -1124,7 +1267,7 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="5"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>3003640</v>
       </c>
@@ -1153,7 +1296,7 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="5"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>3003649</v>
       </c>
@@ -1182,7 +1325,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="5"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>3006759</v>
       </c>
@@ -1211,34 +1354,22 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="5"/>
     </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O19" s="5"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="12"/>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O20" s="5"/>
       <c r="Q20" s="7"/>
       <c r="R20" s="5"/>
     </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="12"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I21" s="10"/>
       <c r="O21" s="5"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="12"/>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I22" s="10"/>
       <c r="N22">
         <v>3003197</v>
@@ -1252,20 +1383,14 @@
       </c>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="12"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I23" s="10"/>
       <c r="Q23" s="7"/>
       <c r="R23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="12"/>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="N24">
         <v>3003198</v>
       </c>
@@ -1276,31 +1401,28 @@
         <v>3000022</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O25" s="5"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="5"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O26" s="5"/>
       <c r="Q26" s="7"/>
       <c r="R26" s="5"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I27" s="10"/>
       <c r="O27" s="5"/>
       <c r="Q27" s="7"/>
       <c r="R27" s="5"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I28" s="10"/>
       <c r="O28" s="5"/>
       <c r="R28" s="5"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I29" s="10"/>
       <c r="N29">
         <v>3003640</v>
@@ -1314,7 +1436,7 @@
       </c>
       <c r="R29" s="5"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I30" s="10"/>
       <c r="N30">
         <v>3003641</v>
@@ -1328,7 +1450,7 @@
       </c>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I31" s="10"/>
       <c r="O31" t="s">
         <v>1</v>
@@ -1338,19 +1460,19 @@
         <v>3003640</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O32" t="s">
         <v>1</v>
       </c>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="8:18">
+    <row r="33" spans="8:18" x14ac:dyDescent="0.2">
       <c r="O33" t="s">
         <v>1</v>
       </c>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="8:18">
+    <row r="34" spans="8:18" x14ac:dyDescent="0.2">
       <c r="H34" s="9" t="s">
         <v>14</v>
       </c>
@@ -1359,7 +1481,7 @@
       </c>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="8:18">
+    <row r="35" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I35" s="10"/>
       <c r="N35">
         <v>3003646</v>
@@ -1367,17 +1489,17 @@
       <c r="O35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="8:18">
+    <row r="36" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I36" s="10"/>
       <c r="O36" s="5"/>
       <c r="R36" s="5"/>
     </row>
-    <row r="37" spans="8:18">
+    <row r="37" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I37" s="10"/>
       <c r="O37" s="5"/>
       <c r="R37" s="5"/>
     </row>
-    <row r="38" spans="8:18">
+    <row r="38" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I38" s="10"/>
       <c r="N38">
         <v>3003649</v>
@@ -1391,35 +1513,35 @@
       </c>
       <c r="R38" s="6"/>
     </row>
-    <row r="39" spans="8:18">
+    <row r="39" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I39" s="10"/>
       <c r="O39" t="s">
         <v>1</v>
       </c>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="8:18">
+    <row r="40" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I40" s="10"/>
       <c r="O40" t="s">
         <v>1</v>
       </c>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="8:18">
+    <row r="41" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I41" s="10"/>
       <c r="O41" t="s">
         <v>1</v>
       </c>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="8:18">
+    <row r="42" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I42" s="10"/>
       <c r="O42" t="s">
         <v>3</v>
       </c>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="8:18">
+    <row r="43" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I43" s="10"/>
       <c r="N43">
         <v>3003654</v>
@@ -1428,29 +1550,29 @@
       <c r="Q43" s="7"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="8:18">
+    <row r="44" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I44" s="10"/>
       <c r="O44" s="5"/>
       <c r="Q44" s="7"/>
       <c r="R44" s="5"/>
     </row>
-    <row r="45" spans="8:18">
+    <row r="45" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I45" s="10"/>
       <c r="O45" s="5"/>
       <c r="Q45" s="7"/>
       <c r="R45" s="5"/>
     </row>
-    <row r="46" spans="8:18">
+    <row r="46" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I46" s="10"/>
       <c r="O46" s="5"/>
       <c r="R46" s="5"/>
     </row>
-    <row r="47" spans="8:18">
+    <row r="47" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I47" s="10"/>
       <c r="O47" s="5"/>
       <c r="R47" s="5"/>
     </row>
-    <row r="48" spans="8:18">
+    <row r="48" spans="8:18" x14ac:dyDescent="0.2">
       <c r="I48" s="10"/>
       <c r="N48">
         <v>3006759</v>
@@ -1464,7 +1586,7 @@
       </c>
       <c r="R48" s="5"/>
     </row>
-    <row r="49" spans="9:18">
+    <row r="49" spans="9:18" x14ac:dyDescent="0.2">
       <c r="I49" s="10"/>
       <c r="N49">
         <v>3006760</v>
@@ -1478,7 +1600,7 @@
       </c>
       <c r="R49" s="5"/>
     </row>
-    <row r="50" spans="9:18">
+    <row r="50" spans="9:18" x14ac:dyDescent="0.2">
       <c r="I50" s="10"/>
       <c r="N50">
         <v>3006761</v>
@@ -1492,7 +1614,7 @@
       </c>
       <c r="R50" s="5"/>
     </row>
-    <row r="51" spans="9:18">
+    <row r="51" spans="9:18" x14ac:dyDescent="0.2">
       <c r="I51" s="10"/>
       <c r="N51">
         <v>3006762</v>
@@ -1506,7 +1628,7 @@
       </c>
       <c r="R51" s="5"/>
     </row>
-    <row r="52" spans="9:18">
+    <row r="52" spans="9:18" x14ac:dyDescent="0.2">
       <c r="I52" s="10"/>
       <c r="N52">
         <v>3006763</v>
@@ -1520,23 +1642,23 @@
       </c>
       <c r="R52" s="6"/>
     </row>
-    <row r="53" spans="9:18">
+    <row r="53" spans="9:18" x14ac:dyDescent="0.2">
       <c r="O53" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="9:18">
+    <row r="54" spans="9:18" x14ac:dyDescent="0.2">
       <c r="O54" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="9:18">
+    <row r="55" spans="9:18" x14ac:dyDescent="0.2">
       <c r="O55" s="4"/>
     </row>
-    <row r="56" spans="9:18">
+    <row r="56" spans="9:18" x14ac:dyDescent="0.2">
       <c r="O56" s="5"/>
     </row>
-    <row r="57" spans="9:18">
+    <row r="57" spans="9:18" x14ac:dyDescent="0.2">
       <c r="O57" s="6"/>
     </row>
   </sheetData>
@@ -1554,4 +1676,1180 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF94AAC-9191-A04C-B2E1-C9A40C2900DD}">
+  <dimension ref="A1:R75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" s="12"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J6" s="13"/>
+      <c r="N6" s="13"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>3007272</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>3007274</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>3028957</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>21683</v>
+      </c>
+      <c r="G8">
+        <f>F8+F7</f>
+        <v>3028957</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>3043837</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="N9" s="13"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>3051722</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10">
+        <v>22773</v>
+      </c>
+      <c r="G10">
+        <f>G8+F10</f>
+        <v>3051730</v>
+      </c>
+      <c r="I10">
+        <v>3007272</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>3007272</v>
+      </c>
+      <c r="N10" s="13"/>
+      <c r="O10" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>3054917</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>3187</v>
+      </c>
+      <c r="G11">
+        <f>G10+F11</f>
+        <v>3054917</v>
+      </c>
+      <c r="I11">
+        <f>I10+1</f>
+        <v>3007273</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>3007273</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <f t="shared" ref="I12:I15" si="0">I11+1</f>
+        <v>3007274</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>3007274</v>
+      </c>
+      <c r="N12" s="14"/>
+      <c r="O12" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J13" s="15"/>
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13">
+        <v>3007275</v>
+      </c>
+      <c r="N13" s="15"/>
+      <c r="O13" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J14" s="15"/>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14">
+        <v>3007276</v>
+      </c>
+      <c r="N14" s="15"/>
+      <c r="O14" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15">
+        <f>I12+1</f>
+        <v>3007275</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>3007277</v>
+      </c>
+      <c r="N15" s="12"/>
+      <c r="O15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <f>I15+1</f>
+        <v>3007276</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="K16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <f>M15+1</f>
+        <v>3007278</v>
+      </c>
+      <c r="N16" s="13"/>
+      <c r="O16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17">
+        <f>I16+1</f>
+        <v>3007277</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17:M29" si="1">M16+1</f>
+        <v>3007279</v>
+      </c>
+      <c r="N17" s="13"/>
+      <c r="O17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>3007272</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18">
+        <f>I17+1</f>
+        <v>3007278</v>
+      </c>
+      <c r="J18" s="13"/>
+      <c r="K18" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>3007280</v>
+      </c>
+      <c r="N18" s="13"/>
+      <c r="O18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>3028959</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19:I29" si="2">I18+1</f>
+        <v>3007279</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>3007281</v>
+      </c>
+      <c r="N19" s="13"/>
+      <c r="O19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>3043840</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>3007280</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>3007282</v>
+      </c>
+      <c r="N20" s="13"/>
+      <c r="O20" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20">
+        <v>1.23456789012345E+19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>3051725</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>3007281</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="K21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>3007283</v>
+      </c>
+      <c r="N21" s="13"/>
+      <c r="O21" t="s">
+        <v>2</v>
+      </c>
+      <c r="R21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>3054924</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>3007282</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" t="s">
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>3007284</v>
+      </c>
+      <c r="N22" s="13"/>
+      <c r="O22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>3007283</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" t="s">
+        <v>3</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>3007285</v>
+      </c>
+      <c r="N23" s="13"/>
+      <c r="O23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>3007284</v>
+      </c>
+      <c r="J24" s="13"/>
+      <c r="K24" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>3007286</v>
+      </c>
+      <c r="N24" s="13"/>
+      <c r="O24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>3007285</v>
+      </c>
+      <c r="J25" s="13"/>
+      <c r="K25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>3007287</v>
+      </c>
+      <c r="N25" s="13"/>
+      <c r="O25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>3007286</v>
+      </c>
+      <c r="J26" s="13"/>
+      <c r="K26" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>3007288</v>
+      </c>
+      <c r="N26" s="13"/>
+      <c r="O26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>3007287</v>
+      </c>
+      <c r="J27" s="13"/>
+      <c r="K27" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>3007289</v>
+      </c>
+      <c r="N27" s="13"/>
+      <c r="O27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>3007288</v>
+      </c>
+      <c r="J28" s="13"/>
+      <c r="K28" t="s">
+        <v>3</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>3007290</v>
+      </c>
+      <c r="N28" s="13"/>
+      <c r="O28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>3007289</v>
+      </c>
+      <c r="J29" s="13"/>
+      <c r="K29" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>3007291</v>
+      </c>
+      <c r="N29" s="13"/>
+      <c r="O29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J30" s="13"/>
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J31" s="13"/>
+      <c r="N31" s="13"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J32" s="13"/>
+      <c r="N32" s="13"/>
+    </row>
+    <row r="33" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J33" s="13"/>
+      <c r="N33" s="13"/>
+    </row>
+    <row r="34" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J34" s="13"/>
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <v>3028956</v>
+      </c>
+      <c r="J35" s="13"/>
+      <c r="K35" t="s">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>3028958</v>
+      </c>
+      <c r="N35" s="13"/>
+      <c r="O35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I36">
+        <v>3028957</v>
+      </c>
+      <c r="J36" s="14"/>
+      <c r="K36" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>3028959</v>
+      </c>
+      <c r="N36" s="14"/>
+      <c r="O36" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="L37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M37">
+        <v>3028960</v>
+      </c>
+      <c r="O37" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I38">
+        <v>3028958</v>
+      </c>
+      <c r="J38" s="12"/>
+      <c r="K38" t="s">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>3028961</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="O38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I39">
+        <v>3028959</v>
+      </c>
+      <c r="J39" s="13"/>
+      <c r="K39" t="s">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>3028962</v>
+      </c>
+      <c r="N39" s="13"/>
+      <c r="O39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J40" s="13"/>
+      <c r="N40" s="13"/>
+    </row>
+    <row r="41" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J41" s="13"/>
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I42">
+        <v>3043835</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" t="s">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>3043838</v>
+      </c>
+      <c r="N42" s="13"/>
+      <c r="O42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I43">
+        <v>3043836</v>
+      </c>
+      <c r="J43" s="14"/>
+      <c r="K43" t="s">
+        <v>2</v>
+      </c>
+      <c r="M43">
+        <v>3043839</v>
+      </c>
+      <c r="N43" s="14"/>
+      <c r="O43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I44">
+        <v>3043837</v>
+      </c>
+      <c r="K44" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="L44" t="s">
+        <v>27</v>
+      </c>
+      <c r="M44">
+        <v>3043840</v>
+      </c>
+      <c r="O44" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I45">
+        <v>3043838</v>
+      </c>
+      <c r="J45" s="12"/>
+      <c r="K45" t="s">
+        <v>3</v>
+      </c>
+      <c r="M45">
+        <v>3043841</v>
+      </c>
+      <c r="N45" s="12"/>
+      <c r="O45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I46">
+        <f>I45+1</f>
+        <v>3043839</v>
+      </c>
+      <c r="J46" s="13"/>
+      <c r="K46" t="s">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f>M45+1</f>
+        <v>3043842</v>
+      </c>
+      <c r="N46" s="13"/>
+      <c r="O46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J47" s="13"/>
+      <c r="N47" s="13"/>
+    </row>
+    <row r="48" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J48" s="13"/>
+      <c r="N48" s="13"/>
+    </row>
+    <row r="49" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I49">
+        <v>3051722</v>
+      </c>
+      <c r="J49" s="13"/>
+      <c r="K49" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M49">
+        <v>3051725</v>
+      </c>
+      <c r="N49" s="13"/>
+      <c r="O49" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I50">
+        <f>I49+1</f>
+        <v>3051723</v>
+      </c>
+      <c r="J50" s="13"/>
+      <c r="K50" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M50">
+        <f>M49+1</f>
+        <v>3051726</v>
+      </c>
+      <c r="N50" s="13"/>
+      <c r="O50" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I51">
+        <f t="shared" ref="I51:I57" si="3">I50+1</f>
+        <v>3051724</v>
+      </c>
+      <c r="J51" s="13"/>
+      <c r="K51" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M51">
+        <f t="shared" ref="M51:M63" si="4">M50+1</f>
+        <v>3051727</v>
+      </c>
+      <c r="N51" s="13"/>
+      <c r="O51" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I52">
+        <f t="shared" si="3"/>
+        <v>3051725</v>
+      </c>
+      <c r="J52" s="13"/>
+      <c r="K52" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="4"/>
+        <v>3051728</v>
+      </c>
+      <c r="N52" s="13"/>
+      <c r="O52" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I53">
+        <f t="shared" si="3"/>
+        <v>3051726</v>
+      </c>
+      <c r="J53" s="13"/>
+      <c r="K53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="4"/>
+        <v>3051729</v>
+      </c>
+      <c r="N53" s="13"/>
+      <c r="O53" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I54">
+        <f t="shared" si="3"/>
+        <v>3051727</v>
+      </c>
+      <c r="J54" s="13"/>
+      <c r="K54" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="4"/>
+        <v>3051730</v>
+      </c>
+      <c r="N54" s="13"/>
+      <c r="O54" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I55">
+        <f t="shared" si="3"/>
+        <v>3051728</v>
+      </c>
+      <c r="J55" s="13"/>
+      <c r="K55" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="4"/>
+        <v>3051731</v>
+      </c>
+      <c r="N55" s="13"/>
+      <c r="O55" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I56">
+        <f t="shared" si="3"/>
+        <v>3051729</v>
+      </c>
+      <c r="J56" s="13"/>
+      <c r="K56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="4"/>
+        <v>3051732</v>
+      </c>
+      <c r="N56" s="13"/>
+      <c r="O56" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I57">
+        <f t="shared" si="3"/>
+        <v>3051730</v>
+      </c>
+      <c r="J57" s="14"/>
+      <c r="K57" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="4"/>
+        <v>3051733</v>
+      </c>
+      <c r="N57" s="14"/>
+      <c r="O57" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="L58" t="s">
+        <v>28</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="4"/>
+        <v>3051734</v>
+      </c>
+      <c r="O58" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="L59" t="s">
+        <v>28</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="4"/>
+        <v>3051735</v>
+      </c>
+      <c r="O59" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="L60" t="s">
+        <v>28</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="4"/>
+        <v>3051736</v>
+      </c>
+      <c r="O60" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="L61" t="s">
+        <v>28</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="4"/>
+        <v>3051737</v>
+      </c>
+      <c r="O61" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I62">
+        <v>3051731</v>
+      </c>
+      <c r="J62" s="12"/>
+      <c r="K62" t="s">
+        <v>3</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="4"/>
+        <v>3051738</v>
+      </c>
+      <c r="N62" s="12"/>
+      <c r="O62" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I63">
+        <v>3051732</v>
+      </c>
+      <c r="J63" s="13"/>
+      <c r="K63" t="s">
+        <v>3</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="4"/>
+        <v>3051739</v>
+      </c>
+      <c r="N63" s="13"/>
+      <c r="O63" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I64">
+        <f>I63+1</f>
+        <v>3051733</v>
+      </c>
+      <c r="J64" s="13"/>
+      <c r="K64" t="s">
+        <v>2</v>
+      </c>
+      <c r="M64">
+        <f>M63+1</f>
+        <v>3051740</v>
+      </c>
+      <c r="N64" s="13"/>
+      <c r="O64" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J65" s="13"/>
+      <c r="N65" s="13"/>
+    </row>
+    <row r="66" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J66" s="13"/>
+      <c r="N66" s="13"/>
+    </row>
+    <row r="67" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I67">
+        <v>3054916</v>
+      </c>
+      <c r="J67" s="13"/>
+      <c r="K67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <v>3054923</v>
+      </c>
+      <c r="N67" s="13"/>
+      <c r="O67" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I68">
+        <v>3054917</v>
+      </c>
+      <c r="J68" s="14"/>
+      <c r="K68" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <v>3054924</v>
+      </c>
+      <c r="N68" s="14"/>
+      <c r="O68" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I69">
+        <v>3054918</v>
+      </c>
+      <c r="K69" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I70">
+        <v>3054919</v>
+      </c>
+      <c r="J70" s="12"/>
+      <c r="K70" t="s">
+        <v>2</v>
+      </c>
+      <c r="M70">
+        <v>3054925</v>
+      </c>
+      <c r="N70" s="12"/>
+      <c r="O70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I71">
+        <v>3054920</v>
+      </c>
+      <c r="J71" s="13"/>
+      <c r="K71" t="s">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <f>M70+1</f>
+        <v>3054926</v>
+      </c>
+      <c r="N71" s="13"/>
+      <c r="O71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J72" s="13"/>
+      <c r="N72" s="13"/>
+    </row>
+    <row r="73" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J73" s="13"/>
+      <c r="N73" s="13"/>
+    </row>
+    <row r="74" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J74" s="13"/>
+      <c r="N74" s="13"/>
+    </row>
+    <row r="75" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J75" s="14"/>
+      <c r="N75" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>